<commit_message>
Login: update qr code image
</commit_message>
<xml_diff>
--- a/lib/samples/assets/csv/form_stories.xlsx
+++ b/lib/samples/assets/csv/form_stories.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="277">
   <si>
     <t>code</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>f1_qu_001||=||other</t>
+  </si>
+  <si>
+    <t>other_country.mp3</t>
   </si>
   <si>
     <t>f1_qu_002</t>
@@ -228,6 +231,9 @@
   </si>
   <si>
     <t>f2_qu_001||=||other</t>
+  </si>
+  <si>
+    <t>other_transportation.mp3</t>
   </si>
   <si>
     <t>f2_qu_002</t>
@@ -1397,7 +1403,9 @@
       <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I3" s="7"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1423,19 +1431,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="2"/>
@@ -1462,10 +1470,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>28</v>
@@ -1474,7 +1482,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="2"/>
@@ -1501,10 +1509,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>28</v>
@@ -1512,10 +1520,10 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="2"/>
@@ -1542,10 +1550,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>28</v>
@@ -1553,10 +1561,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="2"/>
@@ -1583,10 +1591,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>28</v>
@@ -1595,7 +1603,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="2"/>
@@ -1622,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>28</v>
@@ -1634,7 +1642,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="2"/>
@@ -1661,13 +1669,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1677,16 +1685,16 @@
         <v>3.0</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1708,10 +1716,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
@@ -1720,7 +1728,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="2"/>
@@ -1776,10 +1784,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>28</v>
@@ -1788,7 +1796,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="2"/>
@@ -1815,10 +1823,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>32</v>
@@ -1826,9 +1834,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="I14" s="7"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1854,19 +1864,19 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="2"/>
@@ -1893,10 +1903,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>28</v>
@@ -1905,7 +1915,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="2"/>
@@ -1932,10 +1942,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>28</v>
@@ -1944,7 +1954,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="2"/>
@@ -1971,21 +1981,21 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="2"/>
@@ -2012,10 +2022,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>28</v>
@@ -2023,10 +2033,10 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="2"/>
@@ -2053,23 +2063,23 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="2"/>
@@ -2125,10 +2135,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>28</v>
@@ -2137,7 +2147,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="2"/>
@@ -2164,19 +2174,19 @@
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="2"/>
@@ -2203,10 +2213,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>28</v>
@@ -2215,7 +2225,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="2"/>
@@ -2242,19 +2252,19 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="2"/>
@@ -30578,31 +30588,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -30629,14 +30639,14 @@
         <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -30667,14 +30677,14 @@
         <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -30705,14 +30715,14 @@
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -30743,14 +30753,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -30781,14 +30791,14 @@
         <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -30819,14 +30829,14 @@
         <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -30857,14 +30867,14 @@
         <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -30895,14 +30905,14 @@
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -30933,10 +30943,10 @@
         <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -30966,13 +30976,13 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -31002,13 +31012,13 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -31038,13 +31048,13 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -31074,13 +31084,13 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -31110,13 +31120,13 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -31146,13 +31156,13 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -31182,13 +31192,13 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -31218,13 +31228,13 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -31254,13 +31264,13 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -31290,13 +31300,13 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -31326,13 +31336,13 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -31362,13 +31372,13 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -31398,13 +31408,13 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -31434,13 +31444,13 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -31470,13 +31480,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -31506,13 +31516,13 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -31542,13 +31552,13 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -31578,13 +31588,13 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -31614,13 +31624,13 @@
     </row>
     <row r="29">
       <c r="A29" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D29" s="16">
         <v>2.0</v>
@@ -31652,13 +31662,13 @@
     </row>
     <row r="30">
       <c r="A30" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -31688,13 +31698,13 @@
     </row>
     <row r="31">
       <c r="A31" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D31" s="16">
         <v>1.0</v>
@@ -31726,13 +31736,13 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D32" s="16">
         <v>3.0</v>
@@ -31764,13 +31774,13 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D33" s="16">
         <v>2.0</v>
@@ -31802,13 +31812,13 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D34" s="16">
         <v>1.0</v>
@@ -31840,13 +31850,13 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -31876,13 +31886,13 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -31912,13 +31922,13 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -31978,13 +31988,13 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -32014,13 +32024,13 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -32050,13 +32060,13 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -32086,13 +32096,13 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D42" s="16">
         <v>1.0</v>
@@ -32124,13 +32134,13 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D43" s="16">
         <v>1.0</v>
@@ -32162,13 +32172,13 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D44" s="16">
         <v>1.0</v>
@@ -32200,13 +32210,13 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D45" s="16">
         <v>1.0</v>
@@ -32238,13 +32248,13 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D46" s="16">
         <v>1.0</v>
@@ -32276,13 +32286,13 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D47" s="16">
         <v>1.0</v>
@@ -32314,13 +32324,13 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -32350,13 +32360,13 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -32386,13 +32396,13 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -32422,13 +32432,13 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -32458,21 +32468,21 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="6"/>
       <c r="F52" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H52" s="17" t="b">
         <v>1</v>
@@ -32502,13 +32512,13 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -32538,21 +32548,21 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="6"/>
       <c r="F54" s="9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H54" s="17" t="b">
         <v>1</v>
@@ -32580,13 +32590,13 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -32616,13 +32626,13 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -32652,13 +32662,13 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D57" s="16">
         <v>1.0</v>
@@ -32690,13 +32700,13 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D58" s="16">
         <v>1.0</v>
@@ -32728,13 +32738,13 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D59" s="16">
         <v>1.0</v>
@@ -32766,21 +32776,21 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="6"/>
       <c r="F60" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H60" s="17" t="b">
         <v>1</v>
@@ -32810,13 +32820,13 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -32846,13 +32856,13 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -32882,13 +32892,13 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -32918,21 +32928,21 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="6"/>
       <c r="F64" s="9" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H64" s="17" t="b">
         <v>1</v>
@@ -32960,13 +32970,13 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -33026,13 +33036,13 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -33062,21 +33072,21 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -33102,13 +33112,13 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -33138,13 +33148,13 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -33174,13 +33184,13 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -33210,21 +33220,21 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -33250,21 +33260,21 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H73" s="17" t="b">
         <v>1</v>
@@ -33292,21 +33302,21 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="6"/>
       <c r="F74" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -33332,21 +33342,21 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -33372,21 +33382,21 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="6"/>
       <c r="F76" s="11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -33412,13 +33422,13 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -33448,13 +33458,13 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -33484,13 +33494,13 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -33520,21 +33530,21 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="H80" s="13" t="b">
         <v>1</v>

</xml_diff>